<commit_message>
added new test to plan
</commit_message>
<xml_diff>
--- a/artifact/plan/Test-plan.xlsx
+++ b/artifact/plan/Test-plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\MyFirstProject\artifact\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\artifact\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="465" windowWidth="51195" windowHeight="31545" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="51195" windowHeight="31545" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>description</t>
   </si>
@@ -126,15 +126,28 @@
   </si>
   <si>
     <t>Scenario</t>
+  </si>
+  <si>
+    <t>description of third plan step</t>
+  </si>
+  <si>
+    <t>baseMethods</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -370,117 +383,120 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="38" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="38" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="38" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -490,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -500,13 +516,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -524,7 +540,52 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF9F9F9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </right>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -874,7 +935,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,13 +955,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
       <c r="F1" s="17" t="s">
         <v>1</v>
       </c>
@@ -912,20 +973,20 @@
       </c>
       <c r="I1" s="28"/>
       <c r="J1" s="14"/>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:13" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
       <c r="F2" s="15" t="s">
         <v>14</v>
       </c>
@@ -933,9 +994,9 @@
       <c r="H2" s="30"/>
       <c r="I2" s="15"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="36"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="37"/>
     </row>
     <row r="3" spans="1:13" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25"/>
@@ -1025,7 +1086,7 @@
       <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="31" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="6"/>
@@ -1046,14 +1107,26 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" s="16" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
+      <c r="F7" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="1"/>
       <c r="K7" s="21"/>
@@ -1713,20 +1786,36 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7:M50 A6:B6 D6:M6 A5:M5">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="11">
+  <conditionalFormatting sqref="A8:M50 A6:B6 D6:M6 A5:M5">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="15">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="beginsWith" dxfId="2" priority="1" operator="beginsWith" text="WARN ">
+  <conditionalFormatting sqref="L1:L6 L8:L1048576">
+    <cfRule type="beginsWith" dxfId="6" priority="5" operator="beginsWith" text="WARN ">
       <formula>LEFT(L1,LEN("WARN "))="WARN "</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="5" priority="6" operator="beginsWith" text="FAIL">
       <formula>LEFT(L1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="7" operator="beginsWith" text="PASS">
+      <formula>LEFT(L1,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:B7 D7:M7">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7">
+    <cfRule type="beginsWith" dxfId="2" priority="1" operator="beginsWith" text="WARN ">
+      <formula>LEFT(L7,LEN("WARN "))="WARN "</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="FAIL">
+      <formula>LEFT(L7,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="3" operator="beginsWith" text="PASS">
-      <formula>LEFT(L1,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(L7,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>